<commit_message>
Updating price policy code
</commit_message>
<xml_diff>
--- a/aimms_model/energy_hub/results/FlatPricing/results_capacities.xlsx
+++ b/aimms_model/energy_hub/results/FlatPricing/results_capacities.xlsx
@@ -17,15 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Elec</t>
   </si>
   <si>
     <t>Heat</t>
-  </si>
-  <si>
-    <t>Electric_boiler</t>
   </si>
   <si>
     <t>Gas_CHP</t>
@@ -381,13 +378,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -406,19 +403,16 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -427,16 +421,13 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -447,18 +438,15 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
         <v>1</v>
       </c>
     </row>
@@ -469,13 +457,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -494,19 +482,16 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>11.560693641618496</v>
       </c>
       <c r="C2">
-        <v>2.9479768786127161</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -515,27 +500,24 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1140.0784121337804</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6.7122023568540703</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>5.0999999999999996</v>
+        <v>563.40070657927242</v>
       </c>
       <c r="D3">
-        <v>45.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -544,9 +526,6 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
         <v>0</v>
       </c>
     </row>
@@ -576,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>101.9421710154577</v>
+        <v>897.60282631708935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>